<commit_message>
added search by name
</commit_message>
<xml_diff>
--- a/Calc.xlsx
+++ b/Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Neo4J\Alumni App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79A31A3-4700-4730-ACB0-2F64CE6D091D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7FC9CA-22F3-474A-BA18-4A5E5CF5DB03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3468" yWindow="756" windowWidth="17820" windowHeight="11604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -45,49 +45,19 @@
     <t>bachelor_thesis</t>
   </si>
   <si>
-    <t>Amprenta digitala</t>
-  </si>
-  <si>
     <t>Cutarescu</t>
   </si>
   <si>
-    <t>Arina</t>
-  </si>
-  <si>
-    <t>Ixescu</t>
-  </si>
-  <si>
-    <t>arina.ixescu@gmail.com</t>
-  </si>
-  <si>
-    <t>Neo4j</t>
-  </si>
-  <si>
-    <t>Marin</t>
-  </si>
-  <si>
-    <t>Marinescu</t>
-  </si>
-  <si>
-    <t>marin.marinescu@gmail.com</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>maria.cutarescu@gmail.com</t>
-  </si>
-  <si>
-    <t>Algoritmi genetici</t>
-  </si>
-  <si>
-    <t>3215515441587</t>
-  </si>
-  <si>
-    <t>9874563279874</t>
-  </si>
-  <si>
-    <t>1235987531092</t>
+    <t>3215515848587</t>
+  </si>
+  <si>
+    <t>Alexandru</t>
+  </si>
+  <si>
+    <t>alexandru.cutarescu@gmail.com</t>
+  </si>
+  <si>
+    <t>Angular</t>
   </si>
 </sst>
 </file>
@@ -417,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,71 +424,29 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2">
+        <v>2020</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2">
-        <v>2021</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>2019</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>2020</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{C3979422-C10B-4C19-95F3-D948DDA78FF9}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{D24112A1-3FE8-4518-9FA7-F9AE41346A68}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{555FB328-B0FA-45AF-AEB1-1D8DF3D02EEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>